<commit_message>
1. Dish receiver model is simplified by the U formular. 2. cp is simplified as the T independent variable.
</commit_message>
<xml_diff>
--- a/SolarThermalDesign/Water/CalculationFiles/DishReceiver_U/U.xlsx
+++ b/SolarThermalDesign/Water/CalculationFiles/DishReceiver_U/U.xlsx
@@ -2337,11 +2337,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="92386816"/>
-        <c:axId val="92388352"/>
+        <c:axId val="84093184"/>
+        <c:axId val="84148224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92386816"/>
+        <c:axId val="84093184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000"/>
@@ -2350,12 +2350,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92388352"/>
+        <c:crossAx val="84148224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92388352"/>
+        <c:axId val="84148224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="30"/>
@@ -2364,7 +2364,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92386816"/>
+        <c:crossAx val="84093184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2377,7 +2377,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2394,8 +2394,8 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="9.8237116701875696E-2"/>
-          <c:y val="4.8890357970620996E-2"/>
-          <c:w val="0.74218974457461118"/>
+          <c:y val="4.8890357970621003E-2"/>
+          <c:w val="0.74218974457461129"/>
           <c:h val="0.82636429816587764"/>
         </c:manualLayout>
       </c:layout>
@@ -3552,11 +3552,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="91399680"/>
-        <c:axId val="91406336"/>
+        <c:axId val="85022208"/>
+        <c:axId val="85037056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91399680"/>
+        <c:axId val="85022208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="63"/>
@@ -3585,19 +3585,19 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.46207182638755534"/>
-              <c:y val="0.92808587832068234"/>
+              <c:x val="0.4620718263875554"/>
+              <c:y val="0.92808587832068246"/>
             </c:manualLayout>
           </c:layout>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91406336"/>
+        <c:crossAx val="85037056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91406336"/>
+        <c:axId val="85037056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="63"/>
@@ -3626,14 +3626,14 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="9.7560975609756115E-3"/>
+              <c:x val="9.756097560975615E-3"/>
               <c:y val="0.37683504704340742"/>
             </c:manualLayout>
           </c:layout>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91399680"/>
+        <c:crossAx val="85022208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3646,7 +3646,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3943,8 +3943,8 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="84533632"/>
-        <c:axId val="84535168"/>
+        <c:axId val="92116096"/>
+        <c:axId val="92117632"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -5350,23 +5350,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="84533632"/>
-        <c:axId val="84535168"/>
+        <c:axId val="92116096"/>
+        <c:axId val="92117632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84533632"/>
+        <c:axId val="92116096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84535168"/>
+        <c:crossAx val="92117632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84535168"/>
+        <c:axId val="92117632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="61"/>
@@ -5376,7 +5376,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84533632"/>
+        <c:crossAx val="92116096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5389,7 +5389,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5782,8 +5782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46:F47"/>
+    <sheetView tabSelected="1" topLeftCell="M10" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>